<commit_message>
1. Rozdzielono metody na różne serwisy 2. Poprawiono tworzenie dat 3. Utworzono mapowanie dat i miejscowości na id 4. Zrobiono tworzenie gotowych insertów do bazy danych dla skierbieszowa, labuń oraz gminy Zamość
</commit_message>
<xml_diff>
--- a/Data/GminaZamosc.xlsx
+++ b/Data/GminaZamosc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MargulaMonika\Desktop\HARMONOGRAMY 2026\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RymarzJakub\Desktop\Harmonogramy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6733EED-2BCA-49B6-B62E-E26D0CC6BB14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92960CB9-F249-4A16-9404-E27F3680A15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D1706918-D5CC-421B-8F4D-A1A1EE3AC547}"/>
+    <workbookView xWindow="28680" yWindow="2760" windowWidth="29040" windowHeight="15720" xr2:uid="{D1706918-D5CC-421B-8F4D-A1A1EE3AC547}"/>
   </bookViews>
   <sheets>
     <sheet name="2026" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="41">
   <si>
     <t>Miejscowości</t>
   </si>
@@ -61,12 +61,6 @@
   </si>
   <si>
     <t>VII</t>
-  </si>
-  <si>
-    <t>odpady wielkogabarytowe</t>
-  </si>
-  <si>
-    <t>zużyty sprzęt elektryczny i elektroniczny</t>
   </si>
   <si>
     <t>VIII</t>
@@ -104,15 +98,9 @@
     <t>POJEMNIKI NALEŻY WYSTAWIAĆ NAJPÓŹNIEJ DO GODZ 6:30 W DNIU ODBIORU</t>
   </si>
   <si>
-    <t>bioodpady</t>
-  </si>
-  <si>
     <t>HARMONOGRAM ODBIORU ODPADÓW KOMUNALNYCH ZMIESZANYCH I SELEKTYWNIE ZBIERANYCH                                                           Z TERENU GMINY ZAMOŚĆ NA 2026 rok</t>
   </si>
   <si>
-    <t>zużyta odzież i tekstylia</t>
-  </si>
-  <si>
     <t>7, 21</t>
   </si>
   <si>
@@ -149,9 +137,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>B REJON GZB1, GZB2, GZB3</t>
-  </si>
-  <si>
     <t>GZ1</t>
   </si>
   <si>
@@ -174,13 +159,22 @@
   </si>
   <si>
     <t>GZ8</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,15 +223,6 @@
     </font>
     <font>
       <sz val="10.5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.5"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -500,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -541,9 +526,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -557,28 +539,22 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -613,6 +589,12 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -992,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E444FAB2-40FF-4876-9CA0-9FC59B75EF2F}">
-  <dimension ref="A1:N78"/>
+  <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="145" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:A66"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A59" zoomScale="145" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1011,22 +993,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="42" customHeight="1">
-      <c r="A1" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
+      <c r="A1" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="2" spans="1:14" ht="17.25" customHeight="1">
       <c r="A2" s="4" t="s">
@@ -1057,27 +1039,27 @@
         <v>8</v>
       </c>
       <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A3" s="24" t="s">
-        <v>35</v>
+      <c r="A3" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3" s="11">
         <v>14</v>
@@ -1117,9 +1099,9 @@
       </c>
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A4" s="21"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C4" s="11">
         <v>14</v>
@@ -1149,9 +1131,9 @@
       </c>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A5" s="21"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C5" s="11">
         <v>14</v>
@@ -1185,9 +1167,9 @@
       </c>
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A6" s="21"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="11">
@@ -1215,9 +1197,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A7" s="21"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11">
@@ -1245,9 +1227,9 @@
       </c>
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A8" s="21"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="8" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -1265,9 +1247,9 @@
       <c r="N8" s="11"/>
     </row>
     <row r="9" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A9" s="21"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="10" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -1285,29 +1267,29 @@
       <c r="N9" s="11"/>
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A10" s="21"/>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16">
         <v>21</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17">
-        <v>21</v>
-      </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
     </row>
     <row r="11" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A11" s="22"/>
-      <c r="B11" s="15" t="s">
-        <v>34</v>
+      <c r="A11" s="24"/>
+      <c r="B11" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="C11" s="12">
         <v>12</v>
@@ -1319,25 +1301,25 @@
         <v>5</v>
       </c>
       <c r="F11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="K11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="L11" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="M11" s="12">
         <v>5</v>
@@ -1347,53 +1329,53 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A12" s="20" t="s">
-        <v>36</v>
+      <c r="A12" s="34" t="s">
+        <v>31</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="16">
+        <v>25</v>
+      </c>
+      <c r="C12" s="15">
         <v>15</v>
       </c>
-      <c r="D12" s="16">
+      <c r="D12" s="15">
         <v>10</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="15">
         <v>10</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="15">
         <v>9</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G12" s="15">
         <v>8</v>
       </c>
-      <c r="H12" s="16">
+      <c r="H12" s="15">
         <v>10</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="15">
         <v>10</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="15">
         <v>11</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="15">
         <v>8</v>
       </c>
-      <c r="L12" s="16">
+      <c r="L12" s="15">
         <v>8</v>
       </c>
-      <c r="M12" s="16">
+      <c r="M12" s="15">
         <v>9</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="15">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1">
-      <c r="A13" s="21"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="11">
         <v>15</v>
@@ -1423,9 +1405,9 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A14" s="21"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C14" s="11">
         <v>15</v>
@@ -1459,9 +1441,9 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="21"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13">
@@ -1489,9 +1471,9 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A16" s="21"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11">
@@ -1519,9 +1501,9 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A17" s="21"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="8" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11"/>
@@ -1539,9 +1521,9 @@
       <c r="N17" s="11"/>
     </row>
     <row r="18" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A18" s="21"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="10" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
@@ -1559,29 +1541,29 @@
       <c r="N18" s="11"/>
     </row>
     <row r="19" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A19" s="21"/>
-      <c r="B19" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17">
+      <c r="A19" s="23"/>
+      <c r="B19" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16">
         <v>22</v>
       </c>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
     </row>
     <row r="20" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A20" s="22"/>
-      <c r="B20" s="15" t="s">
-        <v>19</v>
+      <c r="A20" s="24"/>
+      <c r="B20" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="C20" s="12">
         <v>12</v>
@@ -1593,25 +1575,25 @@
         <v>5</v>
       </c>
       <c r="F20" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="K20" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="L20" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K20" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L20" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="M20" s="12">
         <v>5</v>
@@ -1621,11 +1603,11 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A21" s="21" t="s">
-        <v>37</v>
+      <c r="A21" s="23" t="s">
+        <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C21" s="11">
         <v>16</v>
@@ -1665,9 +1647,9 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A22" s="21"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C22" s="11">
         <v>16</v>
@@ -1697,9 +1679,9 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A23" s="21"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C23" s="11">
         <v>16</v>
@@ -1733,9 +1715,9 @@
       </c>
     </row>
     <row r="24" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A24" s="21"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11">
@@ -1763,9 +1745,9 @@
       </c>
     </row>
     <row r="25" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A25" s="21"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11">
@@ -1793,9 +1775,9 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A26" s="21"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="8" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -1813,9 +1795,9 @@
       <c r="N26" s="11"/>
     </row>
     <row r="27" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A27" s="21"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="10" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
@@ -1833,29 +1815,29 @@
       <c r="N27" s="11"/>
     </row>
     <row r="28" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A28" s="21"/>
-      <c r="B28" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17">
+      <c r="A28" s="23"/>
+      <c r="B28" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16">
         <v>27</v>
       </c>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
     </row>
     <row r="29" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A29" s="22"/>
-      <c r="B29" s="15" t="s">
-        <v>19</v>
+      <c r="A29" s="24"/>
+      <c r="B29" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="C29" s="12">
         <v>12</v>
@@ -1867,25 +1849,25 @@
         <v>5</v>
       </c>
       <c r="F29" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J29" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="K29" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="L29" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="I29" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K29" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L29" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="M29" s="12">
         <v>5</v>
@@ -1895,11 +1877,11 @@
       </c>
     </row>
     <row r="30" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A30" s="21" t="s">
-        <v>38</v>
+      <c r="A30" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C30" s="13">
         <v>19</v>
@@ -1939,9 +1921,9 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A31" s="21"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C31" s="13">
         <v>19</v>
@@ -1971,9 +1953,9 @@
       </c>
     </row>
     <row r="32" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A32" s="21"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C32" s="13">
         <v>19</v>
@@ -2007,9 +1989,9 @@
       </c>
     </row>
     <row r="33" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A33" s="21"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="11">
@@ -2037,9 +2019,9 @@
       </c>
     </row>
     <row r="34" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A34" s="21"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11">
@@ -2067,9 +2049,9 @@
       </c>
     </row>
     <row r="35" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A35" s="21"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="8" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
@@ -2087,9 +2069,9 @@
       <c r="N35" s="11"/>
     </row>
     <row r="36" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A36" s="21"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="10" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
@@ -2107,29 +2089,29 @@
       <c r="N36" s="11"/>
     </row>
     <row r="37" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A37" s="21"/>
-      <c r="B37" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17">
+      <c r="A37" s="23"/>
+      <c r="B37" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16">
         <v>1</v>
       </c>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17"/>
-      <c r="N37" s="17"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
     </row>
     <row r="38" spans="1:14" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1">
-      <c r="A38" s="22"/>
-      <c r="B38" s="15" t="s">
-        <v>19</v>
+      <c r="A38" s="24"/>
+      <c r="B38" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="C38" s="12">
         <v>12</v>
@@ -2141,25 +2123,25 @@
         <v>5</v>
       </c>
       <c r="F38" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G38" s="12" t="s">
+      <c r="K38" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H38" s="12" t="s">
+      <c r="L38" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K38" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L38" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="M38" s="12">
         <v>5</v>
@@ -2169,53 +2151,53 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A39" s="20" t="s">
-        <v>39</v>
+      <c r="A39" s="34" t="s">
+        <v>34</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" s="16">
+        <v>25</v>
+      </c>
+      <c r="C39" s="15">
         <v>20</v>
       </c>
-      <c r="D39" s="16">
+      <c r="D39" s="15">
         <v>13</v>
       </c>
-      <c r="E39" s="16">
+      <c r="E39" s="15">
         <v>13</v>
       </c>
-      <c r="F39" s="16">
+      <c r="F39" s="15">
         <v>15</v>
       </c>
-      <c r="G39" s="16">
+      <c r="G39" s="15">
         <v>13</v>
       </c>
-      <c r="H39" s="16">
+      <c r="H39" s="15">
         <v>15</v>
       </c>
-      <c r="I39" s="16">
+      <c r="I39" s="15">
         <v>16</v>
       </c>
-      <c r="J39" s="16">
+      <c r="J39" s="15">
         <v>14</v>
       </c>
-      <c r="K39" s="16">
+      <c r="K39" s="15">
         <v>11</v>
       </c>
-      <c r="L39" s="16">
+      <c r="L39" s="15">
         <v>13</v>
       </c>
-      <c r="M39" s="16">
+      <c r="M39" s="15">
         <v>16</v>
       </c>
-      <c r="N39" s="16">
+      <c r="N39" s="15">
         <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A40" s="21"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C40" s="11">
         <v>20</v>
@@ -2245,9 +2227,9 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A41" s="21"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C41" s="13">
         <v>20</v>
@@ -2281,9 +2263,9 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A42" s="21"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11">
@@ -2311,9 +2293,9 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A43" s="21"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11">
@@ -2341,9 +2323,9 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A44" s="21"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="8" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="11"/>
@@ -2361,9 +2343,9 @@
       <c r="N44" s="11"/>
     </row>
     <row r="45" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A45" s="21"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="10" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11"/>
@@ -2381,29 +2363,29 @@
       <c r="N45" s="11"/>
     </row>
     <row r="46" spans="1:14" ht="17.100000000000001" customHeight="1">
-      <c r="A46" s="21"/>
-      <c r="B46" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17">
+      <c r="A46" s="23"/>
+      <c r="B46" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="16"/>
+      <c r="H46" s="16">
         <v>2</v>
       </c>
-      <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="17"/>
-      <c r="L46" s="17"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="17"/>
+      <c r="I46" s="16"/>
+      <c r="J46" s="16"/>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16"/>
+      <c r="M46" s="16"/>
+      <c r="N46" s="16"/>
     </row>
     <row r="47" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" thickBot="1">
-      <c r="A47" s="22"/>
-      <c r="B47" s="15" t="s">
-        <v>19</v>
+      <c r="A47" s="24"/>
+      <c r="B47" s="14" t="s">
+        <v>40</v>
       </c>
       <c r="C47" s="12">
         <v>12</v>
@@ -2415,25 +2397,25 @@
         <v>5</v>
       </c>
       <c r="F47" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I47" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J47" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G47" s="12" t="s">
+      <c r="K47" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H47" s="12" t="s">
+      <c r="L47" s="12" t="s">
         <v>24</v>
-      </c>
-      <c r="I47" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J47" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K47" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L47" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="M47" s="12">
         <v>5</v>
@@ -2442,170 +2424,156 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="21.75" customHeight="1" thickBot="1">
-      <c r="A48" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G48" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H48" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I48" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J48" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="K48" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="L48" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="M48" s="14" t="s">
+    <row r="48" spans="1:14" ht="16.350000000000001" customHeight="1">
+      <c r="A48" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="15">
+        <v>22</v>
+      </c>
+      <c r="D48" s="15">
+        <v>16</v>
+      </c>
+      <c r="E48" s="15">
+        <v>16</v>
+      </c>
+      <c r="F48" s="15">
+        <v>16</v>
+      </c>
+      <c r="G48" s="15">
         <v>14</v>
       </c>
-      <c r="N48" s="14" t="s">
-        <v>15</v>
+      <c r="H48" s="15">
+        <v>16</v>
+      </c>
+      <c r="I48" s="15">
+        <v>17</v>
+      </c>
+      <c r="J48" s="15">
+        <v>17</v>
+      </c>
+      <c r="K48" s="15">
+        <v>14</v>
+      </c>
+      <c r="L48" s="15">
+        <v>14</v>
+      </c>
+      <c r="M48" s="15">
+        <v>17</v>
+      </c>
+      <c r="N48" s="15">
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A49" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" s="16">
+      <c r="A49" s="20"/>
+      <c r="B49" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="11">
         <v>22</v>
       </c>
-      <c r="D49" s="16">
+      <c r="D49" s="11">
         <v>16</v>
       </c>
-      <c r="E49" s="16">
+      <c r="E49" s="11">
         <v>16</v>
       </c>
-      <c r="F49" s="16">
+      <c r="F49" s="11">
         <v>16</v>
       </c>
-      <c r="G49" s="16">
+      <c r="G49" s="11">
         <v>14</v>
       </c>
-      <c r="H49" s="16">
+      <c r="H49" s="11"/>
+      <c r="I49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
+      <c r="M49" s="11">
+        <v>17</v>
+      </c>
+      <c r="N49" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="16.350000000000001" customHeight="1">
+      <c r="A50" s="20"/>
+      <c r="B50" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="13">
+        <v>22</v>
+      </c>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13">
         <v>16</v>
       </c>
-      <c r="I49" s="16">
-        <v>17</v>
-      </c>
-      <c r="J49" s="16">
-        <v>17</v>
-      </c>
-      <c r="K49" s="16">
-        <v>14</v>
-      </c>
-      <c r="L49" s="16">
-        <v>14</v>
-      </c>
-      <c r="M49" s="16">
-        <v>17</v>
-      </c>
-      <c r="N49" s="16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A50" s="26"/>
-      <c r="B50" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C50" s="11">
-        <v>22</v>
-      </c>
-      <c r="D50" s="11">
-        <v>16</v>
-      </c>
-      <c r="E50" s="11">
-        <v>16</v>
-      </c>
-      <c r="F50" s="11">
+      <c r="F50" s="13">
         <v>16</v>
       </c>
       <c r="G50" s="11">
         <v>14</v>
       </c>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-      <c r="L50" s="11"/>
-      <c r="M50" s="11">
+      <c r="H50" s="13">
+        <v>16</v>
+      </c>
+      <c r="I50" s="13">
         <v>17</v>
       </c>
-      <c r="N50" s="11">
+      <c r="J50" s="13">
+        <v>17</v>
+      </c>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13">
         <v>14</v>
       </c>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13">
+        <v>14</v>
+      </c>
     </row>
     <row r="51" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A51" s="26"/>
-      <c r="B51" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C51" s="13">
-        <v>22</v>
-      </c>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13">
-        <v>16</v>
-      </c>
-      <c r="F51" s="13">
-        <v>16</v>
-      </c>
-      <c r="G51" s="11">
+      <c r="A51" s="20"/>
+      <c r="B51" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11">
+        <v>18</v>
+      </c>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11">
+        <v>10</v>
+      </c>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11">
+        <v>3</v>
+      </c>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11">
+        <v>5</v>
+      </c>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11">
+        <v>5</v>
+      </c>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11">
         <v>14</v>
       </c>
-      <c r="H51" s="13">
-        <v>16</v>
-      </c>
-      <c r="I51" s="13">
-        <v>17</v>
-      </c>
-      <c r="J51" s="13">
-        <v>17</v>
-      </c>
-      <c r="K51" s="13"/>
-      <c r="L51" s="13">
-        <v>14</v>
-      </c>
-      <c r="M51" s="13"/>
-      <c r="N51" s="13">
-        <v>14</v>
-      </c>
     </row>
     <row r="52" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A52" s="26"/>
-      <c r="B52" s="6" t="s">
-        <v>32</v>
+      <c r="A52" s="20"/>
+      <c r="B52" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="C52" s="11"/>
       <c r="D52" s="11">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="11">
@@ -2613,55 +2581,45 @@
       </c>
       <c r="G52" s="11"/>
       <c r="H52" s="11">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="I52" s="11"/>
       <c r="J52" s="11">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="K52" s="11"/>
       <c r="L52" s="11">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="M52" s="11"/>
       <c r="N52" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="16.350000000000001" customHeight="1">
+      <c r="A53" s="20"/>
+      <c r="B53" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11">
         <v>14</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A53" s="26"/>
-      <c r="B53" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C53" s="11"/>
-      <c r="D53" s="11">
-        <v>16</v>
-      </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11">
-        <v>10</v>
-      </c>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11">
-        <v>16</v>
-      </c>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11">
-        <v>17</v>
-      </c>
-      <c r="K53" s="11"/>
-      <c r="L53" s="11">
-        <v>14</v>
-      </c>
+      <c r="L53" s="11"/>
       <c r="M53" s="11"/>
-      <c r="N53" s="11">
-        <v>3</v>
-      </c>
+      <c r="N53" s="11"/>
     </row>
     <row r="54" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A54" s="26"/>
-      <c r="B54" s="8" t="s">
-        <v>9</v>
+      <c r="A54" s="20"/>
+      <c r="B54" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C54" s="11"/>
       <c r="D54" s="11"/>
@@ -2669,103 +2627,125 @@
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
+      <c r="I54" s="11">
+        <v>17</v>
+      </c>
       <c r="J54" s="11"/>
-      <c r="K54" s="11">
-        <v>14</v>
-      </c>
+      <c r="K54" s="11"/>
       <c r="L54" s="11"/>
       <c r="M54" s="11"/>
       <c r="N54" s="11"/>
     </row>
     <row r="55" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A55" s="26"/>
-      <c r="B55" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11">
+      <c r="A55" s="21"/>
+      <c r="B55" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" s="16"/>
+      <c r="D55" s="16"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16">
+        <v>3</v>
+      </c>
+      <c r="I55" s="16"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16"/>
+      <c r="L55" s="16"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16"/>
+    </row>
+    <row r="56" spans="1:14" s="1" customFormat="1" ht="16.350000000000001" customHeight="1" thickBot="1">
+      <c r="A56" s="22"/>
+      <c r="B56" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="12">
+        <v>12</v>
+      </c>
+      <c r="D56" s="12">
+        <v>5</v>
+      </c>
+      <c r="E56" s="12">
+        <v>5</v>
+      </c>
+      <c r="F56" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K56" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L56" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M56" s="12">
+        <v>5</v>
+      </c>
+      <c r="N56" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="16.350000000000001" customHeight="1">
+      <c r="A57" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" s="11">
+        <v>23</v>
+      </c>
+      <c r="D57" s="11">
         <v>17</v>
       </c>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
-    </row>
-    <row r="56" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A56" s="24"/>
-      <c r="B56" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="17"/>
-      <c r="E56" s="17"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17">
-        <v>3</v>
-      </c>
-      <c r="I56" s="17"/>
-      <c r="J56" s="17"/>
-      <c r="K56" s="17"/>
-      <c r="L56" s="17"/>
-      <c r="M56" s="17"/>
-      <c r="N56" s="17"/>
-    </row>
-    <row r="57" spans="1:14" s="1" customFormat="1" ht="16.350000000000001" customHeight="1" thickBot="1">
-      <c r="A57" s="27"/>
-      <c r="B57" s="15" t="s">
+      <c r="E57" s="11">
+        <v>17</v>
+      </c>
+      <c r="F57" s="11">
+        <v>17</v>
+      </c>
+      <c r="G57" s="11">
+        <v>15</v>
+      </c>
+      <c r="H57" s="11">
+        <v>18</v>
+      </c>
+      <c r="I57" s="11">
+        <v>20</v>
+      </c>
+      <c r="J57" s="11">
+        <v>18</v>
+      </c>
+      <c r="K57" s="11">
+        <v>15</v>
+      </c>
+      <c r="L57" s="11">
+        <v>15</v>
+      </c>
+      <c r="M57" s="11">
         <v>19</v>
       </c>
-      <c r="C57" s="12">
-        <v>12</v>
-      </c>
-      <c r="D57" s="12">
-        <v>5</v>
-      </c>
-      <c r="E57" s="12">
-        <v>5</v>
-      </c>
-      <c r="F57" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G57" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H57" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I57" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J57" s="12" t="s">
+      <c r="N57" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="16.350000000000001" customHeight="1">
+      <c r="A58" s="23"/>
+      <c r="B58" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="K57" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L57" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M57" s="12">
-        <v>5</v>
-      </c>
-      <c r="N57" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A58" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C58" s="11">
         <v>23</v>
@@ -2782,21 +2762,11 @@
       <c r="G58" s="11">
         <v>15</v>
       </c>
-      <c r="H58" s="11">
-        <v>18</v>
-      </c>
-      <c r="I58" s="11">
-        <v>20</v>
-      </c>
-      <c r="J58" s="11">
-        <v>18</v>
-      </c>
-      <c r="K58" s="11">
-        <v>15</v>
-      </c>
-      <c r="L58" s="11">
-        <v>15</v>
-      </c>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
       <c r="M58" s="11">
         <v>19</v>
       </c>
@@ -2805,16 +2775,14 @@
       </c>
     </row>
     <row r="59" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A59" s="21"/>
-      <c r="B59" s="9" t="s">
-        <v>30</v>
+      <c r="A59" s="23"/>
+      <c r="B59" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="C59" s="11">
         <v>23</v>
       </c>
-      <c r="D59" s="11">
-        <v>17</v>
-      </c>
+      <c r="D59" s="11"/>
       <c r="E59" s="11">
         <v>17</v>
       </c>
@@ -2824,48 +2792,48 @@
       <c r="G59" s="11">
         <v>15</v>
       </c>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
+      <c r="H59" s="11">
+        <v>18</v>
+      </c>
+      <c r="I59" s="11">
+        <v>20</v>
+      </c>
+      <c r="J59" s="11">
+        <v>18</v>
+      </c>
       <c r="K59" s="11"/>
-      <c r="L59" s="11"/>
-      <c r="M59" s="11">
-        <v>19</v>
-      </c>
+      <c r="L59" s="11">
+        <v>15</v>
+      </c>
+      <c r="M59" s="11"/>
       <c r="N59" s="11">
         <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A60" s="21"/>
-      <c r="B60" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C60" s="11">
-        <v>23</v>
-      </c>
-      <c r="D60" s="11"/>
-      <c r="E60" s="11">
-        <v>17</v>
-      </c>
+      <c r="A60" s="23"/>
+      <c r="B60" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11">
+        <v>18</v>
+      </c>
+      <c r="E60" s="11"/>
       <c r="F60" s="11">
-        <v>17</v>
-      </c>
-      <c r="G60" s="11">
-        <v>15</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G60" s="11"/>
       <c r="H60" s="11">
-        <v>18</v>
-      </c>
-      <c r="I60" s="11">
-        <v>20</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="I60" s="11"/>
       <c r="J60" s="11">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="K60" s="11"/>
       <c r="L60" s="11">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="M60" s="11"/>
       <c r="N60" s="11">
@@ -2873,13 +2841,13 @@
       </c>
     </row>
     <row r="61" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A61" s="21"/>
-      <c r="B61" s="6" t="s">
-        <v>32</v>
+      <c r="A61" s="23"/>
+      <c r="B61" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="C61" s="11"/>
       <c r="D61" s="11">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E61" s="11"/>
       <c r="F61" s="11">
@@ -2887,55 +2855,45 @@
       </c>
       <c r="G61" s="11"/>
       <c r="H61" s="11">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="I61" s="11"/>
       <c r="J61" s="11">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="K61" s="11"/>
       <c r="L61" s="11">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="M61" s="11"/>
       <c r="N61" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="16.350000000000001" customHeight="1">
+      <c r="A62" s="23"/>
+      <c r="B62" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="K62" s="11">
         <v>15</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A62" s="21"/>
-      <c r="B62" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C62" s="11"/>
-      <c r="D62" s="11">
-        <v>17</v>
-      </c>
-      <c r="E62" s="11"/>
-      <c r="F62" s="11">
-        <v>21</v>
-      </c>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11">
-        <v>18</v>
-      </c>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11">
-        <v>18</v>
-      </c>
-      <c r="K62" s="11"/>
-      <c r="L62" s="11">
-        <v>15</v>
-      </c>
+      <c r="L62" s="11"/>
       <c r="M62" s="11"/>
-      <c r="N62" s="11">
-        <v>4</v>
-      </c>
+      <c r="N62" s="11"/>
     </row>
     <row r="63" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A63" s="21"/>
-      <c r="B63" s="8" t="s">
-        <v>9</v>
+      <c r="A63" s="23"/>
+      <c r="B63" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C63" s="11"/>
       <c r="D63" s="11"/>
@@ -2943,103 +2901,125 @@
       <c r="F63" s="11"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
+      <c r="I63" s="11">
+        <v>20</v>
+      </c>
       <c r="J63" s="11"/>
-      <c r="K63" s="11">
-        <v>15</v>
-      </c>
+      <c r="K63" s="11"/>
       <c r="L63" s="11"/>
       <c r="M63" s="11"/>
       <c r="N63" s="11"/>
     </row>
     <row r="64" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A64" s="21"/>
-      <c r="B64" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11">
+      <c r="A64" s="23"/>
+      <c r="B64" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C64" s="16"/>
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16">
+        <v>22</v>
+      </c>
+      <c r="I64" s="16"/>
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
+      <c r="L64" s="16"/>
+      <c r="M64" s="16"/>
+      <c r="N64" s="16"/>
+    </row>
+    <row r="65" spans="1:14" s="1" customFormat="1" ht="16.350000000000001" customHeight="1" thickBot="1">
+      <c r="A65" s="24"/>
+      <c r="B65" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="12">
+        <v>12</v>
+      </c>
+      <c r="D65" s="12">
+        <v>5</v>
+      </c>
+      <c r="E65" s="12">
+        <v>5</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
-      <c r="L64" s="11"/>
-      <c r="M64" s="11"/>
-      <c r="N64" s="11"/>
-    </row>
-    <row r="65" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A65" s="21"/>
-      <c r="B65" s="18" t="s">
+      <c r="I65" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17">
+      <c r="J65" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I65" s="17"/>
-      <c r="J65" s="17"/>
-      <c r="K65" s="17"/>
-      <c r="L65" s="17"/>
-      <c r="M65" s="17"/>
-      <c r="N65" s="17"/>
-    </row>
-    <row r="66" spans="1:14" s="1" customFormat="1" ht="16.350000000000001" customHeight="1" thickBot="1">
-      <c r="A66" s="22"/>
-      <c r="B66" s="15" t="s">
+      <c r="K65" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L65" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M65" s="12">
+        <v>5</v>
+      </c>
+      <c r="N65" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="16.350000000000001" customHeight="1">
+      <c r="A66" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66" s="13">
+        <v>26</v>
+      </c>
+      <c r="D66" s="13">
+        <v>20</v>
+      </c>
+      <c r="E66" s="13">
         <v>19</v>
       </c>
-      <c r="C66" s="12">
-        <v>12</v>
-      </c>
-      <c r="D66" s="12">
-        <v>5</v>
-      </c>
-      <c r="E66" s="12">
-        <v>5</v>
-      </c>
-      <c r="F66" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G66" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H66" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I66" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J66" s="12" t="s">
+      <c r="F66" s="13">
+        <v>20</v>
+      </c>
+      <c r="G66" s="13">
+        <v>18</v>
+      </c>
+      <c r="H66" s="13">
+        <v>19</v>
+      </c>
+      <c r="I66" s="13">
+        <v>21</v>
+      </c>
+      <c r="J66" s="13">
+        <v>20</v>
+      </c>
+      <c r="K66" s="13">
+        <v>17</v>
+      </c>
+      <c r="L66" s="13">
+        <v>16</v>
+      </c>
+      <c r="M66" s="13">
+        <v>20</v>
+      </c>
+      <c r="N66" s="13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="16.350000000000001" customHeight="1">
+      <c r="A67" s="23"/>
+      <c r="B67" s="9" t="s">
         <v>26</v>
-      </c>
-      <c r="K66" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L66" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M66" s="12">
-        <v>5</v>
-      </c>
-      <c r="N66" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A67" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="C67" s="13">
         <v>26</v>
@@ -3056,21 +3036,11 @@
       <c r="G67" s="13">
         <v>18</v>
       </c>
-      <c r="H67" s="13">
-        <v>19</v>
-      </c>
-      <c r="I67" s="13">
-        <v>21</v>
-      </c>
-      <c r="J67" s="13">
-        <v>20</v>
-      </c>
-      <c r="K67" s="13">
-        <v>17</v>
-      </c>
-      <c r="L67" s="13">
-        <v>16</v>
-      </c>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="13"/>
+      <c r="L67" s="13"/>
       <c r="M67" s="13">
         <v>20</v>
       </c>
@@ -3079,16 +3049,14 @@
       </c>
     </row>
     <row r="68" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A68" s="21"/>
-      <c r="B68" s="9" t="s">
-        <v>30</v>
+      <c r="A68" s="23"/>
+      <c r="B68" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="C68" s="13">
         <v>26</v>
       </c>
-      <c r="D68" s="13">
-        <v>20</v>
-      </c>
+      <c r="D68" s="13"/>
       <c r="E68" s="13">
         <v>19</v>
       </c>
@@ -3098,62 +3066,62 @@
       <c r="G68" s="13">
         <v>18</v>
       </c>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="13"/>
+      <c r="H68" s="13">
+        <v>19</v>
+      </c>
+      <c r="I68" s="13">
+        <v>21</v>
+      </c>
+      <c r="J68" s="13">
+        <v>20</v>
+      </c>
       <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13">
-        <v>20</v>
-      </c>
+      <c r="L68" s="13">
+        <v>16</v>
+      </c>
+      <c r="M68" s="13"/>
       <c r="N68" s="13">
         <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A69" s="21"/>
-      <c r="B69" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C69" s="13">
-        <v>26</v>
-      </c>
-      <c r="D69" s="13"/>
-      <c r="E69" s="13">
+      <c r="A69" s="23"/>
+      <c r="B69" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11">
+        <v>18</v>
+      </c>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11">
+        <v>23</v>
+      </c>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11">
+        <v>8</v>
+      </c>
+      <c r="I69" s="11"/>
+      <c r="J69" s="11">
+        <v>6</v>
+      </c>
+      <c r="K69" s="11"/>
+      <c r="L69" s="11">
         <v>19</v>
       </c>
-      <c r="F69" s="13">
-        <v>20</v>
-      </c>
-      <c r="G69" s="13">
-        <v>18</v>
-      </c>
-      <c r="H69" s="13">
-        <v>19</v>
-      </c>
-      <c r="I69" s="13">
-        <v>21</v>
-      </c>
-      <c r="J69" s="13">
-        <v>20</v>
-      </c>
-      <c r="K69" s="13"/>
-      <c r="L69" s="13">
-        <v>16</v>
-      </c>
-      <c r="M69" s="13"/>
-      <c r="N69" s="13">
+      <c r="M69" s="11"/>
+      <c r="N69" s="11">
         <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A70" s="21"/>
-      <c r="B70" s="6" t="s">
-        <v>32</v>
+      <c r="A70" s="23"/>
+      <c r="B70" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="C70" s="11"/>
       <c r="D70" s="11">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E70" s="11"/>
       <c r="F70" s="11">
@@ -3161,55 +3129,45 @@
       </c>
       <c r="G70" s="11"/>
       <c r="H70" s="11">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="I70" s="11"/>
       <c r="J70" s="11">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="K70" s="11"/>
       <c r="L70" s="11">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="M70" s="11"/>
       <c r="N70" s="11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="16.350000000000001" customHeight="1">
+      <c r="A71" s="23"/>
+      <c r="B71" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="11"/>
+      <c r="K71" s="11">
         <v>17</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A71" s="21"/>
-      <c r="B71" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11">
-        <v>20</v>
-      </c>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11">
-        <v>23</v>
-      </c>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11">
-        <v>19</v>
-      </c>
-      <c r="I71" s="11"/>
-      <c r="J71" s="11">
-        <v>20</v>
-      </c>
-      <c r="K71" s="11"/>
-      <c r="L71" s="11">
-        <v>16</v>
-      </c>
+      <c r="L71" s="11"/>
       <c r="M71" s="11"/>
-      <c r="N71" s="11">
-        <v>16</v>
-      </c>
+      <c r="N71" s="11"/>
     </row>
     <row r="72" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A72" s="21"/>
-      <c r="B72" s="8" t="s">
-        <v>9</v>
+      <c r="A72" s="23"/>
+      <c r="B72" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C72" s="11"/>
       <c r="D72" s="11"/>
@@ -3217,100 +3175,98 @@
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
-      <c r="I72" s="11"/>
-      <c r="J72" s="11"/>
-      <c r="K72" s="11">
-        <v>17</v>
-      </c>
+      <c r="I72" s="11">
+        <v>21</v>
+      </c>
+      <c r="J72" s="16"/>
+      <c r="K72" s="11"/>
       <c r="L72" s="11"/>
       <c r="M72" s="11"/>
       <c r="N72" s="11"/>
     </row>
     <row r="73" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A73" s="21"/>
-      <c r="B73" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11">
+      <c r="A73" s="23"/>
+      <c r="B73" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16">
+        <v>22</v>
+      </c>
+      <c r="I73" s="16"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="16"/>
+      <c r="L73" s="16"/>
+      <c r="M73" s="16"/>
+      <c r="N73" s="16"/>
+    </row>
+    <row r="74" spans="1:14" s="1" customFormat="1" ht="16.350000000000001" customHeight="1" thickBot="1">
+      <c r="A74" s="24"/>
+      <c r="B74" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C74" s="12">
+        <v>12</v>
+      </c>
+      <c r="D74" s="12">
+        <v>5</v>
+      </c>
+      <c r="E74" s="12">
+        <v>5</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G74" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H74" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I74" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="J73" s="17"/>
-      <c r="K73" s="11"/>
-      <c r="L73" s="11"/>
-      <c r="M73" s="11"/>
-      <c r="N73" s="11"/>
-    </row>
-    <row r="74" spans="1:14" ht="16.350000000000001" customHeight="1">
-      <c r="A74" s="21"/>
-      <c r="B74" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C74" s="17"/>
-      <c r="D74" s="17"/>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17">
+      <c r="J74" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="I74" s="17"/>
-      <c r="J74" s="19"/>
-      <c r="K74" s="17"/>
-      <c r="L74" s="17"/>
-      <c r="M74" s="17"/>
-      <c r="N74" s="17"/>
-    </row>
-    <row r="75" spans="1:14" s="1" customFormat="1" ht="16.350000000000001" customHeight="1" thickBot="1">
-      <c r="A75" s="22"/>
-      <c r="B75" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C75" s="12">
-        <v>12</v>
-      </c>
-      <c r="D75" s="12">
+      <c r="K74" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L74" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M74" s="12">
         <v>5</v>
       </c>
-      <c r="E75" s="12">
-        <v>5</v>
-      </c>
-      <c r="F75" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="G75" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="H75" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="I75" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="J75" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K75" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L75" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M75" s="12">
-        <v>5</v>
-      </c>
-      <c r="N75" s="12">
+      <c r="N74" s="12">
         <v>4</v>
       </c>
+    </row>
+    <row r="75" spans="1:14">
+      <c r="A75" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B75" s="26"/>
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="26"/>
+      <c r="F75" s="26"/>
+      <c r="G75" s="26"/>
+      <c r="H75" s="26"/>
+      <c r="I75" s="26"/>
+      <c r="J75" s="26"/>
+      <c r="K75" s="26"/>
+      <c r="L75" s="26"/>
+      <c r="M75" s="26"/>
+      <c r="N75" s="27"/>
     </row>
     <row r="76" spans="1:14">
       <c r="A76" s="28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B76" s="29"/>
       <c r="C76" s="29"/>
@@ -3328,7 +3284,7 @@
     </row>
     <row r="77" spans="1:14">
       <c r="A77" s="31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B77" s="32"/>
       <c r="C77" s="32"/>
@@ -3344,38 +3300,20 @@
       <c r="M77" s="32"/>
       <c r="N77" s="33"/>
     </row>
-    <row r="78" spans="1:14">
-      <c r="A78" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B78" s="35"/>
-      <c r="C78" s="35"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="35"/>
-      <c r="F78" s="35"/>
-      <c r="G78" s="35"/>
-      <c r="H78" s="35"/>
-      <c r="I78" s="35"/>
-      <c r="J78" s="35"/>
-      <c r="K78" s="35"/>
-      <c r="L78" s="35"/>
-      <c r="M78" s="35"/>
-      <c r="N78" s="36"/>
-    </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A49:A57"/>
-    <mergeCell ref="A58:A66"/>
-    <mergeCell ref="A67:A75"/>
-    <mergeCell ref="A76:N76"/>
     <mergeCell ref="A77:N77"/>
-    <mergeCell ref="A78:N78"/>
     <mergeCell ref="A39:A47"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A3:A11"/>
     <mergeCell ref="A12:A20"/>
     <mergeCell ref="A21:A29"/>
     <mergeCell ref="A30:A38"/>
+    <mergeCell ref="A48:A56"/>
+    <mergeCell ref="A57:A65"/>
+    <mergeCell ref="A66:A74"/>
+    <mergeCell ref="A75:N75"/>
+    <mergeCell ref="A76:N76"/>
   </mergeCells>
   <pageMargins left="0.14583333333333334" right="0.13541666666666666" top="0.17708333333333334" bottom="9.375E-2" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>